<commit_message>
perbaikan notifikasi di controller barangmasuk uploadExcel
</commit_message>
<xml_diff>
--- a/public/templates/barangmasuk.xlsx
+++ b/public/templates/barangmasuk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-new\htdocs\gudang_apk\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516E6410-4047-4FE8-91E3-9F739D1BAED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62091EDE-BC83-46CD-9FDD-1FA230CB15C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9779995E-7E2F-4D4B-82BF-D8DE632A96D1}"/>
   </bookViews>
@@ -393,7 +393,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,14 +412,8 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -503,46 +497,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -555,41 +514,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -613,6 +537,42 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -742,42 +702,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -849,14 +773,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37C751D9-4A36-4E2D-BE0C-65D4F5809446}" name="Table2" displayName="Table2" ref="A1:E15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A1:E15" xr:uid="{37C751D9-4A36-4E2D-BE0C-65D4F5809446}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37C751D9-4A36-4E2D-BE0C-65D4F5809446}" name="Table2" displayName="Table2" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E2" xr:uid="{37C751D9-4A36-4E2D-BE0C-65D4F5809446}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BA94A4CD-94EA-47F6-BFEC-6E644DD35F74}" name="barang_id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DF71CB37-1F71-4D09-9946-CF668653B030}" name="Keterangan" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{9A8CDF9D-71BB-4D69-BFDF-F1E0EA6B3D7B}" name="serial_number" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{340775D0-7102-4B5F-BDF9-FA0E07055487}" name="Kondisi barang" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{2B4F8605-CDF9-4AA5-BC3D-C875FB43A38B}" name="Kelengkapan" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BA94A4CD-94EA-47F6-BFEC-6E644DD35F74}" name="barang_id" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DF71CB37-1F71-4D09-9946-CF668653B030}" name="Keterangan" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9A8CDF9D-71BB-4D69-BFDF-F1E0EA6B3D7B}" name="serial_number" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{340775D0-7102-4B5F-BDF9-FA0E07055487}" name="Kondisi barang" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{2B4F8605-CDF9-4AA5-BC3D-C875FB43A38B}" name="Kelengkapan" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1159,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046A4941-8FEF-4D6E-98B7-45E373F3D4D5}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,19 +1099,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1198,97 +1122,6 @@
       <c r="D2" s="2"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>